<commit_message>
Checking in all updates
</commit_message>
<xml_diff>
--- a/Accounting/CreateDynamicsEntities/Data/Inputs/Bank Accounts.xlsx
+++ b/Accounting/CreateDynamicsEntities/Data/Inputs/Bank Accounts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cardonis-my.sharepoint.com/personal/rbrowning_cardon_us/Documents/Documents/UiPath/Accounting.CreateDynamicsEntities.Performer/Data/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cardonis-my.sharepoint.com/personal/rbrowning_cardon_us/Documents/Documents/UiPath/Robotic Processes/Corporate/Accounting/CreateDynamicsEntities/Data/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{EC8AD84A-A6A6-486F-8D1B-FF5E4867B8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1F5349FE-D59B-4C56-96B8-8973CA2AB96C}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{EC8AD84A-A6A6-486F-8D1B-FF5E4867B8B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{10CA1018-05DD-4E8F-B6AC-C49FFC528F4F}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="60" windowWidth="21840" windowHeight="38040" xr2:uid="{94F7B235-2B9B-42CD-9DBD-920A1265AE39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="38040" activeTab="1" xr2:uid="{94F7B235-2B9B-42CD-9DBD-920A1265AE39}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank Accounts" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>02</t>
   </si>
   <si>
-    <t>Deposit- Electronic</t>
-  </si>
-  <si>
     <t>Altenheim H&amp;L Property, LLC</t>
   </si>
   <si>
@@ -437,9 +434,6 @@
     <t>06</t>
   </si>
   <si>
-    <t>Transfer-Wire</t>
-  </si>
-  <si>
     <t>Bell Trace H&amp;L LLC</t>
   </si>
   <si>
@@ -1308,6 +1302,12 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Deposit - Electronic</t>
+  </si>
+  <si>
+    <t>Transfer - Wire</t>
   </si>
 </sst>
 </file>
@@ -2090,7 +2090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649395C3-FE9F-4708-8567-CA7404E13EBC}">
   <dimension ref="A1:V104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
@@ -2507,7 +2507,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17">
         <v>1400970218</v>
@@ -2541,19 +2541,19 @@
         <v>77</v>
       </c>
       <c r="Q17" t="s">
+        <v>96</v>
+      </c>
+      <c r="R17" t="s">
+        <v>79</v>
+      </c>
+      <c r="S17" t="s">
         <v>97</v>
-      </c>
-      <c r="R17" t="s">
-        <v>79</v>
-      </c>
-      <c r="S17" t="s">
-        <v>98</v>
       </c>
       <c r="T17" t="s">
         <v>81</v>
       </c>
       <c r="U17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18">
         <v>1401035291</v>
@@ -2595,19 +2595,19 @@
         <v>77</v>
       </c>
       <c r="Q18" t="s">
+        <v>102</v>
+      </c>
+      <c r="R18" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" t="s">
         <v>103</v>
-      </c>
-      <c r="R18" t="s">
-        <v>79</v>
-      </c>
-      <c r="S18" t="s">
-        <v>104</v>
       </c>
       <c r="T18" t="s">
         <v>81</v>
       </c>
       <c r="U18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19">
         <v>1400970205</v>
@@ -2649,19 +2649,19 @@
         <v>77</v>
       </c>
       <c r="Q19" t="s">
+        <v>108</v>
+      </c>
+      <c r="R19" t="s">
+        <v>79</v>
+      </c>
+      <c r="S19" t="s">
         <v>109</v>
-      </c>
-      <c r="R19" t="s">
-        <v>79</v>
-      </c>
-      <c r="S19" t="s">
-        <v>110</v>
       </c>
       <c r="T19" t="s">
         <v>81</v>
       </c>
       <c r="U19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>34</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20">
         <v>1400970195</v>
@@ -2703,19 +2703,19 @@
         <v>77</v>
       </c>
       <c r="Q20" t="s">
+        <v>114</v>
+      </c>
+      <c r="R20" t="s">
+        <v>79</v>
+      </c>
+      <c r="S20" t="s">
         <v>115</v>
-      </c>
-      <c r="R20" t="s">
-        <v>79</v>
-      </c>
-      <c r="S20" t="s">
-        <v>116</v>
       </c>
       <c r="T20" t="s">
         <v>81</v>
       </c>
       <c r="U20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21">
         <v>1401080424</v>
@@ -2757,19 +2757,19 @@
         <v>77</v>
       </c>
       <c r="Q21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="R21" t="s">
         <v>79</v>
       </c>
       <c r="S21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T21" t="s">
         <v>81</v>
       </c>
       <c r="U21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C22">
         <v>1401034522</v>
@@ -2811,19 +2811,19 @@
         <v>77</v>
       </c>
       <c r="Q22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R22" t="s">
         <v>79</v>
       </c>
       <c r="S22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="T22" t="s">
         <v>81</v>
       </c>
       <c r="U22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2831,13 +2831,13 @@
         <v>34</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C23">
         <v>5311958374</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6" t="s">
@@ -2847,10 +2847,10 @@
         <v>37</v>
       </c>
       <c r="H23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J23" t="s">
         <v>76</v>
@@ -2862,22 +2862,22 @@
         <v>42</v>
       </c>
       <c r="P23" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>214</v>
+      </c>
+      <c r="R23" t="s">
+        <v>79</v>
+      </c>
+      <c r="S23" t="s">
+        <v>222</v>
+      </c>
+      <c r="T23" t="s">
         <v>223</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="U23" t="s">
         <v>216</v>
-      </c>
-      <c r="R23" t="s">
-        <v>79</v>
-      </c>
-      <c r="S23" t="s">
-        <v>224</v>
-      </c>
-      <c r="T23" t="s">
-        <v>225</v>
-      </c>
-      <c r="U23" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2885,7 +2885,7 @@
         <v>85</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C24">
         <v>103144284</v>
@@ -2901,7 +2901,7 @@
         <v>37</v>
       </c>
       <c r="H24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I24" t="s">
         <v>89</v>
@@ -2919,19 +2919,19 @@
         <v>91</v>
       </c>
       <c r="Q24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R24" t="s">
         <v>79</v>
       </c>
       <c r="S24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="T24" t="s">
         <v>93</v>
       </c>
       <c r="U24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2939,7 +2939,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C25" s="15">
         <v>1400970302</v>
@@ -2973,19 +2973,19 @@
         <v>77</v>
       </c>
       <c r="Q25" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R25" t="s">
         <v>79</v>
       </c>
       <c r="S25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="T25" t="s">
         <v>81</v>
       </c>
       <c r="U25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>85</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C26">
         <v>103628700</v>
@@ -3009,7 +3009,7 @@
         <v>37</v>
       </c>
       <c r="H26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I26" t="s">
         <v>89</v>
@@ -3027,19 +3027,19 @@
         <v>91</v>
       </c>
       <c r="Q26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R26" t="s">
         <v>79</v>
       </c>
       <c r="S26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="T26" t="s">
         <v>93</v>
       </c>
       <c r="U26" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C27">
         <v>1401080437</v>
@@ -3081,27 +3081,27 @@
         <v>77</v>
       </c>
       <c r="Q27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R27" t="s">
         <v>79</v>
       </c>
       <c r="S27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="T27" t="s">
         <v>81</v>
       </c>
       <c r="U27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C28">
         <v>1401260914</v>
@@ -3135,19 +3135,19 @@
         <v>77</v>
       </c>
       <c r="Q28" t="s">
+        <v>247</v>
+      </c>
+      <c r="R28" t="s">
+        <v>248</v>
+      </c>
+      <c r="S28" t="s">
         <v>249</v>
       </c>
-      <c r="R28" t="s">
+      <c r="T28" t="s">
         <v>250</v>
       </c>
-      <c r="S28" t="s">
+      <c r="U28" t="s">
         <v>251</v>
-      </c>
-      <c r="T28" t="s">
-        <v>252</v>
-      </c>
-      <c r="U28" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -3155,7 +3155,7 @@
         <v>34</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C29">
         <v>1400969944</v>
@@ -3189,19 +3189,19 @@
         <v>77</v>
       </c>
       <c r="Q29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R29" t="s">
         <v>79</v>
       </c>
       <c r="S29" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T29" t="s">
         <v>81</v>
       </c>
       <c r="U29" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -3209,7 +3209,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C30">
         <v>103143877</v>
@@ -3225,7 +3225,7 @@
         <v>37</v>
       </c>
       <c r="H30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I30" t="s">
         <v>89</v>
@@ -3243,19 +3243,19 @@
         <v>91</v>
       </c>
       <c r="Q30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="S30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="T30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U30" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C31">
         <v>4318537</v>
@@ -3279,7 +3279,7 @@
         <v>37</v>
       </c>
       <c r="H31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I31" t="s">
         <v>89</v>
@@ -3297,19 +3297,19 @@
         <v>91</v>
       </c>
       <c r="Q31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R31" t="s">
         <v>79</v>
       </c>
       <c r="S31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T31" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U31" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -3317,13 +3317,13 @@
         <v>34</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C32">
         <v>5313830886</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6" t="s">
@@ -3333,10 +3333,10 @@
         <v>37</v>
       </c>
       <c r="H32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J32" t="s">
         <v>76</v>
@@ -3348,22 +3348,22 @@
         <v>42</v>
       </c>
       <c r="P32" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>247</v>
+      </c>
+      <c r="R32" t="s">
+        <v>79</v>
+      </c>
+      <c r="S32" t="s">
+        <v>258</v>
+      </c>
+      <c r="T32" t="s">
         <v>223</v>
       </c>
-      <c r="Q32" t="s">
-        <v>249</v>
-      </c>
-      <c r="R32" t="s">
-        <v>79</v>
-      </c>
-      <c r="S32" t="s">
-        <v>260</v>
-      </c>
-      <c r="T32" t="s">
-        <v>225</v>
-      </c>
       <c r="U32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3371,13 +3371,13 @@
         <v>34</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C33">
         <v>7656757049</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6" t="s">
@@ -3387,10 +3387,10 @@
         <v>37</v>
       </c>
       <c r="H33" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J33" t="s">
         <v>76</v>
@@ -3402,22 +3402,22 @@
         <v>42</v>
       </c>
       <c r="P33" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>247</v>
+      </c>
+      <c r="R33" t="s">
+        <v>79</v>
+      </c>
+      <c r="S33" t="s">
+        <v>264</v>
+      </c>
+      <c r="T33" t="s">
         <v>265</v>
       </c>
-      <c r="Q33" t="s">
-        <v>249</v>
-      </c>
-      <c r="R33" t="s">
-        <v>79</v>
-      </c>
-      <c r="S33" t="s">
-        <v>266</v>
-      </c>
-      <c r="T33" t="s">
-        <v>267</v>
-      </c>
       <c r="U33" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>84</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C34" s="22">
         <v>1400969876</v>
@@ -3459,19 +3459,19 @@
         <v>77</v>
       </c>
       <c r="Q34" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="S34" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="T34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U34" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -3479,7 +3479,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C35">
         <v>1400969892</v>
@@ -3513,19 +3513,19 @@
         <v>77</v>
       </c>
       <c r="Q35" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R35" t="s">
         <v>79</v>
       </c>
       <c r="S35" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T35" t="s">
         <v>81</v>
       </c>
       <c r="U35" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3533,7 +3533,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C36">
         <v>1400970166</v>
@@ -3567,19 +3567,19 @@
         <v>77</v>
       </c>
       <c r="Q36" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R36" t="s">
         <v>79</v>
       </c>
       <c r="S36" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="T36" t="s">
         <v>81</v>
       </c>
       <c r="U36" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3587,7 +3587,7 @@
         <v>85</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C37">
         <v>103628766</v>
@@ -3603,7 +3603,7 @@
         <v>37</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I37" s="26" t="s">
         <v>89</v>
@@ -3621,19 +3621,19 @@
         <v>91</v>
       </c>
       <c r="Q37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R37" t="s">
         <v>79</v>
       </c>
       <c r="S37" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="T37" t="s">
         <v>93</v>
       </c>
       <c r="U37" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C38">
         <v>1401012816</v>
@@ -3675,19 +3675,19 @@
         <v>77</v>
       </c>
       <c r="Q38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R38" t="s">
         <v>79</v>
       </c>
       <c r="S38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="T38" t="s">
         <v>81</v>
       </c>
       <c r="U38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -3803,7 +3803,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C41">
         <v>1400970140</v>
@@ -3837,19 +3837,19 @@
         <v>77</v>
       </c>
       <c r="Q41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R41" t="s">
         <v>79</v>
       </c>
       <c r="S41" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="T41" t="s">
         <v>81</v>
       </c>
       <c r="U41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -3857,7 +3857,7 @@
         <v>34</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C42">
         <v>1400970111</v>
@@ -3891,19 +3891,19 @@
         <v>77</v>
       </c>
       <c r="Q42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="R42" t="s">
         <v>79</v>
       </c>
       <c r="S42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="T42" t="s">
         <v>81</v>
       </c>
       <c r="U42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -3911,13 +3911,13 @@
         <v>34</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C43">
         <v>1016317442</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="6" t="s">
@@ -3927,10 +3927,10 @@
         <v>37</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J43" s="24" t="s">
         <v>90</v>
@@ -3942,22 +3942,22 @@
         <v>42</v>
       </c>
       <c r="P43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q43" t="s">
+        <v>392</v>
+      </c>
+      <c r="R43" t="s">
+        <v>79</v>
+      </c>
+      <c r="S43" t="s">
+        <v>393</v>
+      </c>
+      <c r="T43" t="s">
+        <v>165</v>
+      </c>
+      <c r="U43" t="s">
         <v>394</v>
-      </c>
-      <c r="R43" t="s">
-        <v>79</v>
-      </c>
-      <c r="S43" t="s">
-        <v>395</v>
-      </c>
-      <c r="T43" t="s">
-        <v>167</v>
-      </c>
-      <c r="U43" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -3965,7 +3965,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C44">
         <v>128496590</v>
@@ -3981,7 +3981,7 @@
         <v>37</v>
       </c>
       <c r="H44" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I44" s="25" t="s">
         <v>89</v>
@@ -3999,19 +3999,19 @@
         <v>91</v>
       </c>
       <c r="Q44" t="s">
+        <v>392</v>
+      </c>
+      <c r="R44" t="s">
+        <v>79</v>
+      </c>
+      <c r="S44" t="s">
+        <v>395</v>
+      </c>
+      <c r="T44" t="s">
+        <v>255</v>
+      </c>
+      <c r="U44" t="s">
         <v>394</v>
-      </c>
-      <c r="R44" t="s">
-        <v>79</v>
-      </c>
-      <c r="S44" t="s">
-        <v>397</v>
-      </c>
-      <c r="T44" t="s">
-        <v>257</v>
-      </c>
-      <c r="U44" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -4019,7 +4019,7 @@
         <v>34</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C45">
         <v>1400970108</v>
@@ -4053,19 +4053,19 @@
         <v>77</v>
       </c>
       <c r="Q45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R45" t="s">
         <v>79</v>
       </c>
       <c r="S45" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="T45" t="s">
         <v>81</v>
       </c>
       <c r="U45" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
         <v>34</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C46" s="20">
         <v>1401129000</v>
@@ -4107,19 +4107,19 @@
         <v>77</v>
       </c>
       <c r="Q46" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="R46" t="s">
         <v>79</v>
       </c>
       <c r="S46" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="T46" t="s">
         <v>81</v>
       </c>
       <c r="U46" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -4127,7 +4127,7 @@
         <v>34</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C47">
         <v>1400969889</v>
@@ -4161,19 +4161,19 @@
         <v>77</v>
       </c>
       <c r="Q47" t="s">
+        <v>271</v>
+      </c>
+      <c r="R47" t="s">
+        <v>272</v>
+      </c>
+      <c r="S47" t="s">
         <v>273</v>
-      </c>
-      <c r="R47" t="s">
-        <v>274</v>
-      </c>
-      <c r="S47" t="s">
-        <v>275</v>
       </c>
       <c r="T47" t="s">
         <v>81</v>
       </c>
       <c r="U47" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -4181,7 +4181,7 @@
         <v>34</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C48">
         <v>103628359</v>
@@ -4197,7 +4197,7 @@
         <v>37</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I48" s="25" t="s">
         <v>89</v>
@@ -4215,19 +4215,19 @@
         <v>91</v>
       </c>
       <c r="Q48" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="R48" t="s">
         <v>79</v>
       </c>
       <c r="S48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="T48" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="U48" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
@@ -4235,7 +4235,7 @@
         <v>34</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C49">
         <v>1401271165</v>
@@ -4269,19 +4269,19 @@
         <v>77</v>
       </c>
       <c r="Q49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R49" t="s">
         <v>79</v>
       </c>
       <c r="S49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="T49" t="s">
         <v>81</v>
       </c>
       <c r="U49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
         <v>34</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C50">
         <v>1401127125</v>
@@ -4323,19 +4323,19 @@
         <v>77</v>
       </c>
       <c r="Q50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R50" t="s">
         <v>79</v>
       </c>
       <c r="S50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="T50" t="s">
         <v>81</v>
       </c>
       <c r="U50" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
@@ -4343,13 +4343,13 @@
         <v>34</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C51">
         <v>1016050446</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6" t="s">
@@ -4359,10 +4359,10 @@
         <v>37</v>
       </c>
       <c r="H51" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J51" t="s">
         <v>90</v>
@@ -4374,22 +4374,22 @@
         <v>42</v>
       </c>
       <c r="P51" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>163</v>
+      </c>
+      <c r="R51" t="s">
+        <v>79</v>
+      </c>
+      <c r="S51" t="s">
         <v>164</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="T51" t="s">
         <v>165</v>
       </c>
-      <c r="R51" t="s">
-        <v>79</v>
-      </c>
-      <c r="S51" t="s">
+      <c r="U51" t="s">
         <v>166</v>
-      </c>
-      <c r="T51" t="s">
-        <v>167</v>
-      </c>
-      <c r="U51" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
@@ -4397,7 +4397,7 @@
         <v>34</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C52">
         <v>123276908</v>
@@ -4413,7 +4413,7 @@
         <v>37</v>
       </c>
       <c r="H52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I52" t="s">
         <v>89</v>
@@ -4431,19 +4431,19 @@
         <v>91</v>
       </c>
       <c r="Q52" t="s">
+        <v>381</v>
+      </c>
+      <c r="R52" t="s">
+        <v>79</v>
+      </c>
+      <c r="S52" t="s">
+        <v>382</v>
+      </c>
+      <c r="T52" t="s">
+        <v>255</v>
+      </c>
+      <c r="U52" t="s">
         <v>383</v>
-      </c>
-      <c r="R52" t="s">
-        <v>79</v>
-      </c>
-      <c r="S52" t="s">
-        <v>384</v>
-      </c>
-      <c r="T52" t="s">
-        <v>257</v>
-      </c>
-      <c r="U52" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
@@ -4451,7 +4451,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C53">
         <v>1401271013</v>
@@ -4485,27 +4485,27 @@
         <v>77</v>
       </c>
       <c r="Q53" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="R53" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="S53" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="T53" t="s">
         <v>81</v>
       </c>
       <c r="U53" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C54">
         <v>1401159229</v>
@@ -4539,19 +4539,19 @@
         <v>77</v>
       </c>
       <c r="Q54" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="R54" t="s">
         <v>79</v>
       </c>
       <c r="S54" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="T54" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="U54" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -4559,7 +4559,7 @@
         <v>34</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C55">
         <v>1400997068</v>
@@ -4593,19 +4593,19 @@
         <v>77</v>
       </c>
       <c r="Q55" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="R55" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="S55" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="T55" t="s">
         <v>81</v>
       </c>
       <c r="U55" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
@@ -4613,7 +4613,7 @@
         <v>34</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C56">
         <v>1400969931</v>
@@ -4647,19 +4647,19 @@
         <v>77</v>
       </c>
       <c r="Q56" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="R56" t="s">
         <v>79</v>
       </c>
       <c r="S56" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="T56" t="s">
         <v>81</v>
       </c>
       <c r="U56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
@@ -4667,7 +4667,7 @@
         <v>34</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C57">
         <v>1400970098</v>
@@ -4701,19 +4701,19 @@
         <v>77</v>
       </c>
       <c r="Q57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R57" t="s">
         <v>79</v>
       </c>
       <c r="S57" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="T57" t="s">
         <v>81</v>
       </c>
       <c r="U57" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
@@ -4721,7 +4721,7 @@
         <v>34</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C58">
         <v>1401220611</v>
@@ -4755,19 +4755,19 @@
         <v>77</v>
       </c>
       <c r="Q58" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R58" t="s">
         <v>79</v>
       </c>
       <c r="S58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="T58" t="s">
         <v>81</v>
       </c>
       <c r="U58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
@@ -4775,7 +4775,7 @@
         <v>34</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C59">
         <v>1400970263</v>
@@ -4809,19 +4809,19 @@
         <v>77</v>
       </c>
       <c r="Q59" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="R59" t="s">
         <v>79</v>
       </c>
       <c r="S59" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="T59" t="s">
         <v>81</v>
       </c>
       <c r="U59" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
@@ -4829,7 +4829,7 @@
         <v>34</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C60">
         <v>1400970247</v>
@@ -4863,19 +4863,19 @@
         <v>77</v>
       </c>
       <c r="Q60" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R60" t="s">
         <v>79</v>
       </c>
       <c r="S60" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="T60" t="s">
         <v>81</v>
       </c>
       <c r="U60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
@@ -4883,7 +4883,7 @@
         <v>34</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C61">
         <v>1401168265</v>
@@ -4917,19 +4917,19 @@
         <v>77</v>
       </c>
       <c r="Q61" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="R61" t="s">
         <v>79</v>
       </c>
       <c r="S61" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="T61" t="s">
         <v>81</v>
       </c>
       <c r="U61" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
@@ -4937,7 +4937,7 @@
         <v>34</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C62">
         <v>1400970357</v>
@@ -4971,19 +4971,19 @@
         <v>77</v>
       </c>
       <c r="Q62" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="R62" t="s">
         <v>79</v>
       </c>
       <c r="S62" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="T62" t="s">
         <v>81</v>
       </c>
       <c r="U62" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
         <v>34</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C63">
         <v>1401271204</v>
@@ -5025,19 +5025,19 @@
         <v>77</v>
       </c>
       <c r="Q63" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R63" t="s">
         <v>79</v>
       </c>
       <c r="S63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="T63" t="s">
         <v>81</v>
       </c>
       <c r="U63" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -5045,7 +5045,7 @@
         <v>34</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C64">
         <v>1400970056</v>
@@ -5079,19 +5079,19 @@
         <v>77</v>
       </c>
       <c r="Q64" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R64" t="s">
         <v>79</v>
       </c>
       <c r="S64" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="T64" t="s">
         <v>81</v>
       </c>
       <c r="U64" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
@@ -5099,7 +5099,7 @@
         <v>34</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C65">
         <v>1400970043</v>
@@ -5133,19 +5133,19 @@
         <v>77</v>
       </c>
       <c r="Q65" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="R65" t="s">
         <v>79</v>
       </c>
       <c r="S65" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="T65" t="s">
         <v>81</v>
       </c>
       <c r="U65" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
@@ -5153,7 +5153,7 @@
         <v>34</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C66">
         <v>1401150671</v>
@@ -5187,19 +5187,19 @@
         <v>77</v>
       </c>
       <c r="Q66" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="R66" t="s">
         <v>79</v>
       </c>
       <c r="S66" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="T66" t="s">
         <v>81</v>
       </c>
       <c r="U66" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
@@ -5207,7 +5207,7 @@
         <v>84</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C67">
         <v>1401150684</v>
@@ -5241,19 +5241,19 @@
         <v>77</v>
       </c>
       <c r="Q67" t="s">
+        <v>287</v>
+      </c>
+      <c r="R67" t="s">
+        <v>79</v>
+      </c>
+      <c r="S67" t="s">
+        <v>290</v>
+      </c>
+      <c r="T67" t="s">
+        <v>291</v>
+      </c>
+      <c r="U67" t="s">
         <v>289</v>
-      </c>
-      <c r="R67" t="s">
-        <v>79</v>
-      </c>
-      <c r="S67" t="s">
-        <v>292</v>
-      </c>
-      <c r="T67" t="s">
-        <v>293</v>
-      </c>
-      <c r="U67" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
@@ -5261,7 +5261,7 @@
         <v>34</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C68">
         <v>1401153717</v>
@@ -5295,19 +5295,19 @@
         <v>77</v>
       </c>
       <c r="Q68" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="R68" t="s">
         <v>79</v>
       </c>
       <c r="S68" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="T68" t="s">
         <v>81</v>
       </c>
       <c r="U68" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -5315,7 +5315,7 @@
         <v>84</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C69">
         <v>1401216337</v>
@@ -5349,19 +5349,19 @@
         <v>77</v>
       </c>
       <c r="Q69" t="s">
+        <v>293</v>
+      </c>
+      <c r="R69" t="s">
+        <v>79</v>
+      </c>
+      <c r="S69" t="s">
+        <v>296</v>
+      </c>
+      <c r="T69" t="s">
+        <v>291</v>
+      </c>
+      <c r="U69" t="s">
         <v>295</v>
-      </c>
-      <c r="R69" t="s">
-        <v>79</v>
-      </c>
-      <c r="S69" t="s">
-        <v>298</v>
-      </c>
-      <c r="T69" t="s">
-        <v>293</v>
-      </c>
-      <c r="U69" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
@@ -5369,7 +5369,7 @@
         <v>34</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C70">
         <v>1401150697</v>
@@ -5403,19 +5403,19 @@
         <v>77</v>
       </c>
       <c r="Q70" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="R70" t="s">
         <v>79</v>
       </c>
       <c r="S70" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="T70" t="s">
         <v>81</v>
       </c>
       <c r="U70" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
@@ -5423,7 +5423,7 @@
         <v>84</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C71">
         <v>1401150710</v>
@@ -5457,19 +5457,19 @@
         <v>77</v>
       </c>
       <c r="Q71" t="s">
+        <v>298</v>
+      </c>
+      <c r="R71" t="s">
+        <v>79</v>
+      </c>
+      <c r="S71" t="s">
+        <v>301</v>
+      </c>
+      <c r="T71" t="s">
+        <v>291</v>
+      </c>
+      <c r="U71" t="s">
         <v>300</v>
-      </c>
-      <c r="R71" t="s">
-        <v>79</v>
-      </c>
-      <c r="S71" t="s">
-        <v>303</v>
-      </c>
-      <c r="T71" t="s">
-        <v>293</v>
-      </c>
-      <c r="U71" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
@@ -5477,13 +5477,13 @@
         <v>84</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C72">
         <v>100445859</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6" t="s">
@@ -5493,10 +5493,10 @@
         <v>37</v>
       </c>
       <c r="H72" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I72" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J72" t="s">
         <v>90</v>
@@ -5508,22 +5508,22 @@
         <v>42</v>
       </c>
       <c r="P72" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>298</v>
+      </c>
+      <c r="R72" t="s">
+        <v>79</v>
+      </c>
+      <c r="S72" t="s">
+        <v>398</v>
+      </c>
+      <c r="T72" t="s">
         <v>357</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="U72" t="s">
         <v>300</v>
-      </c>
-      <c r="R72" t="s">
-        <v>79</v>
-      </c>
-      <c r="S72" t="s">
-        <v>400</v>
-      </c>
-      <c r="T72" t="s">
-        <v>359</v>
-      </c>
-      <c r="U72" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
@@ -5531,7 +5531,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C73">
         <v>1401150655</v>
@@ -5565,19 +5565,19 @@
         <v>77</v>
       </c>
       <c r="Q73" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="R73" t="s">
         <v>79</v>
       </c>
       <c r="S73" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="T73" t="s">
         <v>81</v>
       </c>
       <c r="U73" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
@@ -5585,13 +5585,13 @@
         <v>84</v>
       </c>
       <c r="B74" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="C74" t="s">
+        <v>307</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="C74" t="s">
-        <v>309</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>310</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6" t="s">
@@ -5601,13 +5601,13 @@
         <v>37</v>
       </c>
       <c r="H74" t="s">
+        <v>309</v>
+      </c>
+      <c r="I74" t="s">
+        <v>310</v>
+      </c>
+      <c r="J74" t="s">
         <v>311</v>
-      </c>
-      <c r="I74" t="s">
-        <v>312</v>
-      </c>
-      <c r="J74" t="s">
-        <v>313</v>
       </c>
       <c r="K74">
         <v>15230</v>
@@ -5616,22 +5616,22 @@
         <v>42</v>
       </c>
       <c r="P74" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>303</v>
+      </c>
+      <c r="R74" t="s">
+        <v>79</v>
+      </c>
+      <c r="S74" t="s">
+        <v>313</v>
+      </c>
+      <c r="T74" t="s">
         <v>314</v>
       </c>
-      <c r="Q74" t="s">
+      <c r="U74" t="s">
         <v>305</v>
-      </c>
-      <c r="R74" t="s">
-        <v>79</v>
-      </c>
-      <c r="S74" t="s">
-        <v>315</v>
-      </c>
-      <c r="T74" t="s">
-        <v>316</v>
-      </c>
-      <c r="U74" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
@@ -5639,7 +5639,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C75" s="18">
         <v>1401153720</v>
@@ -5673,7 +5673,7 @@
         <v>77</v>
       </c>
       <c r="Q75" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R75" t="s">
         <v>79</v>
@@ -5685,7 +5685,7 @@
         <v>81</v>
       </c>
       <c r="U75" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
@@ -5693,7 +5693,7 @@
         <v>84</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C76">
         <v>103144295</v>
@@ -5709,7 +5709,7 @@
         <v>37</v>
       </c>
       <c r="H76" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I76" t="s">
         <v>89</v>
@@ -5727,19 +5727,19 @@
         <v>91</v>
       </c>
       <c r="Q76" t="s">
+        <v>316</v>
+      </c>
+      <c r="R76" t="s">
+        <v>79</v>
+      </c>
+      <c r="S76" t="s">
         <v>318</v>
       </c>
-      <c r="R76" t="s">
-        <v>79</v>
-      </c>
-      <c r="S76" t="s">
-        <v>320</v>
-      </c>
       <c r="T76" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U76" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
@@ -5747,7 +5747,7 @@
         <v>84</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C77">
         <v>1401153733</v>
@@ -5781,19 +5781,19 @@
         <v>77</v>
       </c>
       <c r="Q77" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="R77" t="s">
         <v>79</v>
       </c>
       <c r="S77" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="T77" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U77" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
@@ -5801,7 +5801,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C78" s="18">
         <v>1401159384</v>
@@ -5835,7 +5835,7 @@
         <v>77</v>
       </c>
       <c r="Q78" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="R78" t="s">
         <v>79</v>
@@ -5847,7 +5847,7 @@
         <v>81</v>
       </c>
       <c r="U78" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -5855,7 +5855,7 @@
         <v>84</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C79">
         <v>1401159407</v>
@@ -5889,19 +5889,19 @@
         <v>77</v>
       </c>
       <c r="Q79" t="s">
+        <v>322</v>
+      </c>
+      <c r="R79" t="s">
+        <v>79</v>
+      </c>
+      <c r="S79" t="s">
         <v>324</v>
       </c>
-      <c r="R79" t="s">
-        <v>79</v>
-      </c>
-      <c r="S79" t="s">
-        <v>326</v>
-      </c>
       <c r="T79" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U79" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
@@ -5909,7 +5909,7 @@
         <v>34</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C80" s="18">
         <v>1401153746</v>
@@ -5943,7 +5943,7 @@
         <v>77</v>
       </c>
       <c r="Q80" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="R80" t="s">
         <v>79</v>
@@ -5955,7 +5955,7 @@
         <v>81</v>
       </c>
       <c r="U80" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
@@ -5963,7 +5963,7 @@
         <v>34</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C81" s="18">
         <v>1401150639</v>
@@ -5997,19 +5997,19 @@
         <v>77</v>
       </c>
       <c r="Q81" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R81" t="s">
         <v>79</v>
       </c>
       <c r="S81" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="T81" t="s">
         <v>81</v>
       </c>
       <c r="U81" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
@@ -6017,13 +6017,13 @@
         <v>84</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6" t="s">
@@ -6033,13 +6033,13 @@
         <v>37</v>
       </c>
       <c r="H82" t="s">
+        <v>309</v>
+      </c>
+      <c r="I82" t="s">
+        <v>310</v>
+      </c>
+      <c r="J82" t="s">
         <v>311</v>
-      </c>
-      <c r="I82" t="s">
-        <v>312</v>
-      </c>
-      <c r="J82" t="s">
-        <v>313</v>
       </c>
       <c r="K82">
         <v>15230</v>
@@ -6048,22 +6048,22 @@
         <v>42</v>
       </c>
       <c r="P82" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>375</v>
+      </c>
+      <c r="R82" t="s">
+        <v>79</v>
+      </c>
+      <c r="S82" t="s">
+        <v>379</v>
+      </c>
+      <c r="T82" t="s">
         <v>314</v>
       </c>
-      <c r="Q82" t="s">
+      <c r="U82" t="s">
         <v>377</v>
-      </c>
-      <c r="R82" t="s">
-        <v>79</v>
-      </c>
-      <c r="S82" t="s">
-        <v>381</v>
-      </c>
-      <c r="T82" t="s">
-        <v>316</v>
-      </c>
-      <c r="U82" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
@@ -6071,7 +6071,7 @@
         <v>34</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C83" s="18">
         <v>1401153759</v>
@@ -6105,7 +6105,7 @@
         <v>77</v>
       </c>
       <c r="Q83" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="R83" t="s">
         <v>79</v>
@@ -6117,7 +6117,7 @@
         <v>81</v>
       </c>
       <c r="U83" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
@@ -6125,7 +6125,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C84">
         <v>1401216609</v>
@@ -6159,19 +6159,19 @@
         <v>77</v>
       </c>
       <c r="Q84" t="s">
+        <v>329</v>
+      </c>
+      <c r="R84" t="s">
+        <v>79</v>
+      </c>
+      <c r="S84" t="s">
         <v>331</v>
       </c>
-      <c r="R84" t="s">
-        <v>79</v>
-      </c>
-      <c r="S84" t="s">
-        <v>333</v>
-      </c>
       <c r="T84" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U84" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
@@ -6179,7 +6179,7 @@
         <v>34</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C85" s="18">
         <v>1401153762</v>
@@ -6213,19 +6213,19 @@
         <v>77</v>
       </c>
       <c r="Q85" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="R85" t="s">
         <v>79</v>
       </c>
       <c r="S85" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="T85" t="s">
         <v>81</v>
       </c>
       <c r="U85" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
@@ -6233,7 +6233,7 @@
         <v>34</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C86" s="18">
         <v>1401159290</v>
@@ -6267,19 +6267,19 @@
         <v>77</v>
       </c>
       <c r="Q86" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="R86" t="s">
         <v>79</v>
       </c>
       <c r="S86" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="T86" t="s">
         <v>81</v>
       </c>
       <c r="U86" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6287,7 +6287,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C87">
         <v>1401159313</v>
@@ -6321,19 +6321,19 @@
         <v>77</v>
       </c>
       <c r="Q87" t="s">
+        <v>337</v>
+      </c>
+      <c r="R87" t="s">
+        <v>79</v>
+      </c>
+      <c r="S87" t="s">
+        <v>340</v>
+      </c>
+      <c r="T87" t="s">
+        <v>291</v>
+      </c>
+      <c r="U87" t="s">
         <v>339</v>
-      </c>
-      <c r="R87" t="s">
-        <v>79</v>
-      </c>
-      <c r="S87" t="s">
-        <v>342</v>
-      </c>
-      <c r="T87" t="s">
-        <v>293</v>
-      </c>
-      <c r="U87" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
@@ -6341,7 +6341,7 @@
         <v>34</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C88" s="18">
         <v>1401217789</v>
@@ -6375,19 +6375,19 @@
         <v>77</v>
       </c>
       <c r="Q88" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="R88" t="s">
         <v>79</v>
       </c>
       <c r="S88" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="T88" t="s">
         <v>81</v>
       </c>
       <c r="U88" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -6395,13 +6395,13 @@
         <v>84</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C89" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E89" s="6"/>
       <c r="F89" s="6" t="s">
@@ -6411,13 +6411,13 @@
         <v>37</v>
       </c>
       <c r="H89" t="s">
+        <v>309</v>
+      </c>
+      <c r="I89" t="s">
+        <v>310</v>
+      </c>
+      <c r="J89" t="s">
         <v>311</v>
-      </c>
-      <c r="I89" t="s">
-        <v>312</v>
-      </c>
-      <c r="J89" t="s">
-        <v>313</v>
       </c>
       <c r="K89">
         <v>15230</v>
@@ -6426,22 +6426,22 @@
         <v>42</v>
       </c>
       <c r="P89" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>342</v>
+      </c>
+      <c r="R89" t="s">
+        <v>79</v>
+      </c>
+      <c r="S89" t="s">
+        <v>346</v>
+      </c>
+      <c r="T89" t="s">
         <v>314</v>
       </c>
-      <c r="Q89" t="s">
+      <c r="U89" t="s">
         <v>344</v>
-      </c>
-      <c r="R89" t="s">
-        <v>79</v>
-      </c>
-      <c r="S89" t="s">
-        <v>348</v>
-      </c>
-      <c r="T89" t="s">
-        <v>316</v>
-      </c>
-      <c r="U89" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
@@ -6449,7 +6449,7 @@
         <v>34</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C90" s="18">
         <v>1401166665</v>
@@ -6483,19 +6483,19 @@
         <v>77</v>
       </c>
       <c r="Q90" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="R90" t="s">
         <v>79</v>
       </c>
       <c r="S90" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="T90" t="s">
         <v>81</v>
       </c>
       <c r="U90" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
@@ -6503,7 +6503,7 @@
         <v>84</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C91">
         <v>1401216599</v>
@@ -6537,19 +6537,19 @@
         <v>77</v>
       </c>
       <c r="Q91" t="s">
+        <v>348</v>
+      </c>
+      <c r="R91" t="s">
+        <v>79</v>
+      </c>
+      <c r="S91" t="s">
+        <v>351</v>
+      </c>
+      <c r="T91" t="s">
+        <v>291</v>
+      </c>
+      <c r="U91" t="s">
         <v>350</v>
-      </c>
-      <c r="R91" t="s">
-        <v>79</v>
-      </c>
-      <c r="S91" t="s">
-        <v>353</v>
-      </c>
-      <c r="T91" t="s">
-        <v>293</v>
-      </c>
-      <c r="U91" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
@@ -6557,13 +6557,13 @@
         <v>84</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C92">
         <v>560161093</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E92" s="6"/>
       <c r="F92" s="6" t="s">
@@ -6573,10 +6573,10 @@
         <v>37</v>
       </c>
       <c r="H92" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I92" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J92" t="s">
         <v>90</v>
@@ -6588,22 +6588,22 @@
         <v>42</v>
       </c>
       <c r="P92" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>348</v>
+      </c>
+      <c r="R92" t="s">
+        <v>79</v>
+      </c>
+      <c r="S92" t="s">
+        <v>356</v>
+      </c>
+      <c r="T92" t="s">
         <v>357</v>
       </c>
-      <c r="Q92" t="s">
+      <c r="U92" t="s">
         <v>350</v>
-      </c>
-      <c r="R92" t="s">
-        <v>79</v>
-      </c>
-      <c r="S92" t="s">
-        <v>358</v>
-      </c>
-      <c r="T92" t="s">
-        <v>359</v>
-      </c>
-      <c r="U92" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -6611,7 +6611,7 @@
         <v>34</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C93" s="18">
         <v>1401159342</v>
@@ -6645,19 +6645,19 @@
         <v>77</v>
       </c>
       <c r="Q93" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R93" t="s">
         <v>79</v>
       </c>
       <c r="S93" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="T93" t="s">
         <v>81</v>
       </c>
       <c r="U93" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
@@ -6665,7 +6665,7 @@
         <v>84</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C94">
         <v>103628711</v>
@@ -6681,7 +6681,7 @@
         <v>37</v>
       </c>
       <c r="H94" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I94" t="s">
         <v>89</v>
@@ -6699,19 +6699,19 @@
         <v>91</v>
       </c>
       <c r="Q94" t="s">
+        <v>359</v>
+      </c>
+      <c r="R94" t="s">
+        <v>79</v>
+      </c>
+      <c r="S94" t="s">
+        <v>362</v>
+      </c>
+      <c r="T94" t="s">
+        <v>319</v>
+      </c>
+      <c r="U94" t="s">
         <v>361</v>
-      </c>
-      <c r="R94" t="s">
-        <v>79</v>
-      </c>
-      <c r="S94" t="s">
-        <v>364</v>
-      </c>
-      <c r="T94" t="s">
-        <v>321</v>
-      </c>
-      <c r="U94" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
@@ -6719,7 +6719,7 @@
         <v>84</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C95" s="20">
         <v>1401159355</v>
@@ -6753,19 +6753,19 @@
         <v>77</v>
       </c>
       <c r="Q95" t="s">
+        <v>359</v>
+      </c>
+      <c r="R95" t="s">
+        <v>79</v>
+      </c>
+      <c r="S95" t="s">
+        <v>403</v>
+      </c>
+      <c r="T95" t="s">
+        <v>291</v>
+      </c>
+      <c r="U95" t="s">
         <v>361</v>
-      </c>
-      <c r="R95" t="s">
-        <v>79</v>
-      </c>
-      <c r="S95" t="s">
-        <v>405</v>
-      </c>
-      <c r="T95" t="s">
-        <v>293</v>
-      </c>
-      <c r="U95" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
@@ -6773,7 +6773,7 @@
         <v>34</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C96" s="18">
         <v>1401159258</v>
@@ -6807,33 +6807,33 @@
         <v>77</v>
       </c>
       <c r="Q96" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="R96" t="s">
         <v>79</v>
       </c>
       <c r="S96" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="T96" t="s">
         <v>81</v>
       </c>
       <c r="U96" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C97">
         <v>100445697</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E97" s="6"/>
       <c r="F97" s="6" t="s">
@@ -6843,10 +6843,10 @@
         <v>37</v>
       </c>
       <c r="H97" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I97" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J97" t="s">
         <v>90</v>
@@ -6858,22 +6858,22 @@
         <v>42</v>
       </c>
       <c r="P97" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="Q97" t="s">
+        <v>364</v>
+      </c>
+      <c r="R97" t="s">
+        <v>79</v>
+      </c>
+      <c r="S97" t="s">
+        <v>368</v>
+      </c>
+      <c r="T97" t="s">
+        <v>369</v>
+      </c>
+      <c r="U97" t="s">
         <v>366</v>
-      </c>
-      <c r="R97" t="s">
-        <v>79</v>
-      </c>
-      <c r="S97" t="s">
-        <v>370</v>
-      </c>
-      <c r="T97" t="s">
-        <v>371</v>
-      </c>
-      <c r="U97" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
@@ -6881,13 +6881,13 @@
         <v>84</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C98" s="20">
         <v>1401159261</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E98" s="6"/>
       <c r="F98" s="6" t="s">
@@ -6915,19 +6915,19 @@
         <v>77</v>
       </c>
       <c r="Q98" t="s">
+        <v>364</v>
+      </c>
+      <c r="R98" t="s">
+        <v>79</v>
+      </c>
+      <c r="S98" t="s">
+        <v>397</v>
+      </c>
+      <c r="T98" t="s">
+        <v>291</v>
+      </c>
+      <c r="U98" t="s">
         <v>366</v>
-      </c>
-      <c r="R98" t="s">
-        <v>79</v>
-      </c>
-      <c r="S98" t="s">
-        <v>399</v>
-      </c>
-      <c r="T98" t="s">
-        <v>293</v>
-      </c>
-      <c r="U98" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
@@ -6935,7 +6935,7 @@
         <v>34</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C99" s="18">
         <v>1401153788</v>
@@ -6969,19 +6969,19 @@
         <v>77</v>
       </c>
       <c r="Q99" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R99" t="s">
         <v>79</v>
       </c>
       <c r="S99" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="T99" t="s">
         <v>81</v>
       </c>
       <c r="U99" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
@@ -6989,13 +6989,13 @@
         <v>34</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C100">
         <v>1016453052</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E100" s="6"/>
       <c r="F100" s="6" t="s">
@@ -7005,10 +7005,10 @@
         <v>37</v>
       </c>
       <c r="H100" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I100" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J100" s="24" t="s">
         <v>90</v>
@@ -7020,22 +7020,22 @@
         <v>42</v>
       </c>
       <c r="P100" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q100" t="s">
+        <v>387</v>
+      </c>
+      <c r="R100" t="s">
+        <v>79</v>
+      </c>
+      <c r="S100" t="s">
+        <v>388</v>
+      </c>
+      <c r="T100" t="s">
+        <v>165</v>
+      </c>
+      <c r="U100" t="s">
         <v>389</v>
-      </c>
-      <c r="R100" t="s">
-        <v>79</v>
-      </c>
-      <c r="S100" t="s">
-        <v>390</v>
-      </c>
-      <c r="T100" t="s">
-        <v>167</v>
-      </c>
-      <c r="U100" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
@@ -7043,7 +7043,7 @@
         <v>34</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C101">
         <v>121347997</v>
@@ -7059,7 +7059,7 @@
         <v>37</v>
       </c>
       <c r="H101" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I101" s="25" t="s">
         <v>89</v>
@@ -7077,19 +7077,19 @@
         <v>91</v>
       </c>
       <c r="Q101" t="s">
+        <v>387</v>
+      </c>
+      <c r="R101" t="s">
+        <v>79</v>
+      </c>
+      <c r="S101" t="s">
+        <v>390</v>
+      </c>
+      <c r="T101" t="s">
+        <v>255</v>
+      </c>
+      <c r="U101" t="s">
         <v>389</v>
-      </c>
-      <c r="R101" t="s">
-        <v>79</v>
-      </c>
-      <c r="S101" t="s">
-        <v>392</v>
-      </c>
-      <c r="T101" t="s">
-        <v>257</v>
-      </c>
-      <c r="U101" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
@@ -7097,7 +7097,7 @@
         <v>34</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C102">
         <v>1401271194</v>
@@ -7131,19 +7131,19 @@
         <v>77</v>
       </c>
       <c r="Q102" t="s">
+        <v>233</v>
+      </c>
+      <c r="R102" t="s">
+        <v>234</v>
+      </c>
+      <c r="S102" t="s">
         <v>235</v>
-      </c>
-      <c r="R102" t="s">
-        <v>236</v>
-      </c>
-      <c r="S102" t="s">
-        <v>237</v>
       </c>
       <c r="T102" t="s">
         <v>81</v>
       </c>
       <c r="U102" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
@@ -7151,7 +7151,7 @@
         <v>34</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C103">
         <v>1401227834</v>
@@ -7185,19 +7185,19 @@
         <v>77</v>
       </c>
       <c r="Q103" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="R103" t="s">
         <v>79</v>
       </c>
       <c r="S103" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="T103" t="s">
         <v>81</v>
       </c>
       <c r="U103" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
@@ -7205,7 +7205,7 @@
         <v>34</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C104">
         <v>1401271246</v>
@@ -7239,19 +7239,19 @@
         <v>77</v>
       </c>
       <c r="Q104" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="R104" t="s">
         <v>79</v>
       </c>
       <c r="S104" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="T104" t="s">
         <v>81</v>
       </c>
       <c r="U104" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -7277,8 +7277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FC3C61-9B53-47EE-9F0A-4B9495521B22}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7289,10 +7289,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -7308,87 +7308,87 @@
         <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
-      </c>
-      <c r="B4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
         <v>112</v>
-      </c>
-      <c r="B6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -7398,18 +7398,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7591,18 +7591,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5846C49B-2C45-4710-AD5D-4631845C227D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5960D167-8D5B-4D8A-B459-829E2848237F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5960D167-8D5B-4D8A-B459-829E2848237F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5846C49B-2C45-4710-AD5D-4631845C227D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>